<commit_message>
target and test putput removed
</commit_message>
<xml_diff>
--- a/src/test/resources/inputData.xlsx
+++ b/src/test/resources/inputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18030" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13200" windowHeight="6660" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="5" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R32"/>
+  <oleSize ref="A1:M20"/>
 </workbook>
 </file>
 
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>